<commit_message>
small changes to excel files
</commit_message>
<xml_diff>
--- a/ELISA_data/092518 IFNg ELISA Plate2.xlsx
+++ b/ELISA_data/092518 IFNg ELISA Plate2.xlsx
@@ -410,8 +410,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -488,7 +490,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -497,6 +499,7 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -505,6 +508,7 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -775,7 +779,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1720,8 +1724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1760,7 +1764,7 @@
         <v>43368</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
         <v>43</v>
@@ -1783,7 +1787,7 @@
         <v>43368</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
         <v>44</v>
@@ -1806,7 +1810,7 @@
         <v>43368</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
         <v>45</v>
@@ -1829,7 +1833,7 @@
         <v>43368</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
         <v>46</v>
@@ -1852,7 +1856,7 @@
         <v>43368</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
         <v>47</v>
@@ -1875,7 +1879,7 @@
         <v>43368</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
         <v>48</v>
@@ -1898,7 +1902,7 @@
         <v>43368</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
         <v>49</v>
@@ -1921,7 +1925,7 @@
         <v>43368</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
         <v>50</v>
@@ -1944,7 +1948,7 @@
         <v>43368</v>
       </c>
       <c r="D10">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
         <v>51</v>
@@ -1967,7 +1971,7 @@
         <v>43368</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
         <v>52</v>
@@ -1990,7 +1994,7 @@
         <v>43368</v>
       </c>
       <c r="D12">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
         <v>53</v>
@@ -2013,7 +2017,7 @@
         <v>43368</v>
       </c>
       <c r="D13">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
         <v>54</v>
@@ -2036,7 +2040,7 @@
         <v>43368</v>
       </c>
       <c r="D14">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
         <v>55</v>
@@ -2059,7 +2063,7 @@
         <v>43368</v>
       </c>
       <c r="D15">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="E15" t="s">
         <v>56</v>
@@ -2082,7 +2086,7 @@
         <v>43368</v>
       </c>
       <c r="D16">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
         <v>57</v>
@@ -2105,7 +2109,7 @@
         <v>43368</v>
       </c>
       <c r="D17">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
         <v>58</v>
@@ -2128,7 +2132,7 @@
         <v>43368</v>
       </c>
       <c r="D18">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
         <v>59</v>
@@ -2151,7 +2155,7 @@
         <v>43368</v>
       </c>
       <c r="D19">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
         <v>60</v>
@@ -2174,7 +2178,7 @@
         <v>43368</v>
       </c>
       <c r="D20">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
         <v>61</v>
@@ -2197,7 +2201,7 @@
         <v>43368</v>
       </c>
       <c r="D21">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
         <v>62</v>
@@ -2220,7 +2224,7 @@
         <v>43368</v>
       </c>
       <c r="D22">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s">
         <v>63</v>
@@ -2243,7 +2247,7 @@
         <v>43368</v>
       </c>
       <c r="D23">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s">
         <v>64</v>
@@ -2266,7 +2270,7 @@
         <v>43368</v>
       </c>
       <c r="D24">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
         <v>65</v>
@@ -2289,7 +2293,7 @@
         <v>43368</v>
       </c>
       <c r="D25">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="E25" t="s">
         <v>66</v>
@@ -2312,7 +2316,7 @@
         <v>43368</v>
       </c>
       <c r="D26">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E26" t="s">
         <v>67</v>
@@ -2335,7 +2339,7 @@
         <v>43368</v>
       </c>
       <c r="D27">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="E27" t="s">
         <v>68</v>
@@ -2358,7 +2362,7 @@
         <v>43368</v>
       </c>
       <c r="D28">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="E28" t="s">
         <v>69</v>
@@ -2381,7 +2385,7 @@
         <v>43368</v>
       </c>
       <c r="D29">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="E29" t="s">
         <v>70</v>
@@ -2404,7 +2408,7 @@
         <v>43368</v>
       </c>
       <c r="D30">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="E30" t="s">
         <v>71</v>
@@ -2427,7 +2431,7 @@
         <v>43368</v>
       </c>
       <c r="D31">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="E31" t="s">
         <v>72</v>
@@ -2450,7 +2454,7 @@
         <v>43368</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E32" t="s">
         <v>43</v>
@@ -2473,7 +2477,7 @@
         <v>43368</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E33" t="s">
         <v>44</v>
@@ -2496,7 +2500,7 @@
         <v>43368</v>
       </c>
       <c r="D34">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="E34" t="s">
         <v>45</v>
@@ -2519,7 +2523,7 @@
         <v>43368</v>
       </c>
       <c r="D35">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="E35" t="s">
         <v>46</v>
@@ -2542,7 +2546,7 @@
         <v>43368</v>
       </c>
       <c r="D36">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E36" t="s">
         <v>47</v>
@@ -2565,7 +2569,7 @@
         <v>43368</v>
       </c>
       <c r="D37">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="E37" t="s">
         <v>48</v>
@@ -2588,7 +2592,7 @@
         <v>43368</v>
       </c>
       <c r="D38">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="E38" t="s">
         <v>49</v>
@@ -2611,7 +2615,7 @@
         <v>43368</v>
       </c>
       <c r="D39">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="E39" t="s">
         <v>50</v>
@@ -2634,7 +2638,7 @@
         <v>43368</v>
       </c>
       <c r="D40">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="E40" t="s">
         <v>51</v>
@@ -2657,7 +2661,7 @@
         <v>43368</v>
       </c>
       <c r="D41">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E41" t="s">
         <v>52</v>
@@ -2680,7 +2684,7 @@
         <v>43368</v>
       </c>
       <c r="D42">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="E42" t="s">
         <v>53</v>
@@ -2703,7 +2707,7 @@
         <v>43368</v>
       </c>
       <c r="D43">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="E43" t="s">
         <v>54</v>
@@ -2726,7 +2730,7 @@
         <v>43368</v>
       </c>
       <c r="D44">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="E44" t="s">
         <v>55</v>
@@ -2749,7 +2753,7 @@
         <v>43368</v>
       </c>
       <c r="D45">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="E45" t="s">
         <v>56</v>
@@ -2772,7 +2776,7 @@
         <v>43368</v>
       </c>
       <c r="D46">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="E46" t="s">
         <v>57</v>
@@ -2795,7 +2799,7 @@
         <v>43368</v>
       </c>
       <c r="D47">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="E47" t="s">
         <v>58</v>
@@ -2818,7 +2822,7 @@
         <v>43368</v>
       </c>
       <c r="D48">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="E48" t="s">
         <v>59</v>
@@ -2841,7 +2845,7 @@
         <v>43368</v>
       </c>
       <c r="D49">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="E49" t="s">
         <v>60</v>
@@ -2864,7 +2868,7 @@
         <v>43368</v>
       </c>
       <c r="D50">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="E50" t="s">
         <v>61</v>
@@ -2887,7 +2891,7 @@
         <v>43368</v>
       </c>
       <c r="D51">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E51" t="s">
         <v>62</v>
@@ -2910,7 +2914,7 @@
         <v>43368</v>
       </c>
       <c r="D52">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="E52" t="s">
         <v>63</v>
@@ -2933,7 +2937,7 @@
         <v>43368</v>
       </c>
       <c r="D53">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="E53" t="s">
         <v>64</v>
@@ -2956,7 +2960,7 @@
         <v>43368</v>
       </c>
       <c r="D54">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="E54" t="s">
         <v>65</v>
@@ -2979,7 +2983,7 @@
         <v>43368</v>
       </c>
       <c r="D55">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="E55" t="s">
         <v>66</v>
@@ -3002,7 +3006,7 @@
         <v>43368</v>
       </c>
       <c r="D56">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E56" t="s">
         <v>67</v>
@@ -3025,7 +3029,7 @@
         <v>43368</v>
       </c>
       <c r="D57">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="E57" t="s">
         <v>68</v>
@@ -3048,7 +3052,7 @@
         <v>43368</v>
       </c>
       <c r="D58">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="E58" t="s">
         <v>69</v>
@@ -3071,7 +3075,7 @@
         <v>43368</v>
       </c>
       <c r="D59">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="E59" t="s">
         <v>70</v>
@@ -3094,7 +3098,7 @@
         <v>43368</v>
       </c>
       <c r="D60">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="E60" t="s">
         <v>71</v>
@@ -3117,7 +3121,7 @@
         <v>43368</v>
       </c>
       <c r="D61">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="E61" t="s">
         <v>72</v>
@@ -3131,6 +3135,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>